<commit_message>
added data from excel to model with jena
</commit_message>
<xml_diff>
--- a/sample_file.xlsx
+++ b/sample_file.xlsx
@@ -29,6 +29,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,10 +111,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -129,8 +130,12 @@
         <v>5</v>
       </c>
       <c r="C1" s="0" t="n">
-        <f aca="false">A:A+B:B</f>
+        <f aca="false">A1+B1</f>
         <v>9</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <f aca="false">A1*B1</f>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -141,8 +146,12 @@
         <v>4</v>
       </c>
       <c r="C2" s="0" t="n">
-        <f aca="false">A:A+B:B</f>
+        <f aca="false">A2+B2</f>
         <v>7</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">A2*B2</f>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -153,8 +162,12 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
-        <f aca="false">A:A+B:B</f>
+        <f aca="false">A3+B3</f>
         <v>7</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">A3*B3</f>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -165,8 +178,12 @@
         <v>2</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">A:A+B:B</f>
+        <f aca="false">A4+B4</f>
         <v>6</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">A4*B4</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added formula and range logic
</commit_message>
<xml_diff>
--- a/sample_file.xlsx
+++ b/sample_file.xlsx
@@ -17,6 +17,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
+  <si>
+    <t xml:space="preserve">sample1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample3</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -111,10 +125,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -130,13 +144,26 @@
         <v>5</v>
       </c>
       <c r="C1" s="0" t="n">
-        <f aca="false">A1+B1</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D1" s="0" t="n">
+        <f aca="false">A1*B1*C1</f>
+        <v>60</v>
+      </c>
+      <c r="E1" s="0" t="n">
         <f aca="false">A1*B1</f>
         <v>20</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <f aca="false">SUMPRODUCT((F$1:F$9519=F1)*(G$1:G$9519=G1)*C$2:C$9519)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -146,12 +173,25 @@
         <v>4</v>
       </c>
       <c r="C2" s="0" t="n">
-        <f aca="false">A2+B2</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D2" s="0" t="n">
+        <f aca="false">A2*B2*C2</f>
+        <v>36</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <f aca="false">A2*B2</f>
         <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">SUMPRODUCT((F$1:F$9519=F2)*(G$1:G$9519=G2)*C$2:C$9519)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -162,13 +202,26 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
-        <f aca="false">A3+B3</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="0" t="n">
+        <f aca="false">A3*B3*C3</f>
+        <v>30</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <f aca="false">A3*B3</f>
         <v>6</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">SUMPRODUCT((F$1:F$9519=F3)*(G$1:G$9519=G3)*C$2:C$9519)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -178,12 +231,25 @@
         <v>2</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">A4+B4</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="0" t="n">
+        <f aca="false">A4*B4*C4</f>
+        <v>32</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <f aca="false">A4*B4</f>
         <v>8</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">SUMPRODUCT((F$1:F$9519=F4)*(G$1:G$9519=G4)*C$2:C$9519)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>